<commit_message>
The data is deleted from chapter 1.2 in term 4
</commit_message>
<xml_diff>
--- a/Ver_Year_2/24_TRIM.xlsx
+++ b/Ver_Year_2/24_TRIM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\24-AGR\24-AGR\Version1\Versiunea Anuala\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\24-AGR\24-AGR\Ver_Year_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73EED82F-F2FF-4646-88C0-F111F40ECAC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7314E823-CB33-4E59-8AAB-043367006ECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{270B01E8-BC1B-48F2-A63B-1CB23688CFEC}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{270B01E8-BC1B-48F2-A63B-1CB23688CFEC}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -631,9 +631,6 @@
     <t>dec/DataSet/Data/CAP11_R1_C6</t>
   </si>
   <si>
-    <t>dec/DataSet/Data/CAP11_R11_C8</t>
-  </si>
-  <si>
     <t>dec/DataSet/Data/CAP11_R2_C1</t>
   </si>
   <si>
@@ -1322,6 +1319,9 @@
   </si>
   <si>
     <t>dec/DataSet/Data/CAP12_R11_C1</t>
+  </si>
+  <si>
+    <t>dec/DataSet/Data/CAP11_R1_C8</t>
   </si>
 </sst>
 </file>
@@ -1697,7 +1697,7 @@
   <dimension ref="A1:AH145"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3208,7 +3208,7 @@
         <v>126</v>
       </c>
       <c r="C23" t="s">
-        <v>203</v>
+        <v>433</v>
       </c>
       <c r="F23" t="s">
         <v>82</v>
@@ -3270,7 +3270,7 @@
         <v>127</v>
       </c>
       <c r="C24" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F24" t="s">
         <v>82</v>
@@ -3332,7 +3332,7 @@
         <v>128</v>
       </c>
       <c r="C25" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F25" t="s">
         <v>82</v>
@@ -3394,7 +3394,7 @@
         <v>129</v>
       </c>
       <c r="C26" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F26" t="s">
         <v>82</v>
@@ -3456,7 +3456,7 @@
         <v>130</v>
       </c>
       <c r="C27" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F27" t="s">
         <v>82</v>
@@ -3518,7 +3518,7 @@
         <v>131</v>
       </c>
       <c r="C28" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F28" t="s">
         <v>82</v>
@@ -3580,7 +3580,7 @@
         <v>132</v>
       </c>
       <c r="C29" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F29" t="s">
         <v>82</v>
@@ -3642,7 +3642,7 @@
         <v>133</v>
       </c>
       <c r="C30" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F30" t="s">
         <v>82</v>
@@ -3704,7 +3704,7 @@
         <v>134</v>
       </c>
       <c r="C31" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F31" t="s">
         <v>82</v>
@@ -3766,7 +3766,7 @@
         <v>135</v>
       </c>
       <c r="C32" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F32" t="s">
         <v>82</v>
@@ -3828,7 +3828,7 @@
         <v>136</v>
       </c>
       <c r="C33" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F33" t="s">
         <v>82</v>
@@ -3890,7 +3890,7 @@
         <v>137</v>
       </c>
       <c r="C34" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F34" t="s">
         <v>82</v>
@@ -3952,7 +3952,7 @@
         <v>138</v>
       </c>
       <c r="C35" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F35" t="s">
         <v>82</v>
@@ -4014,7 +4014,7 @@
         <v>139</v>
       </c>
       <c r="C36" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F36" t="s">
         <v>82</v>
@@ -4076,7 +4076,7 @@
         <v>140</v>
       </c>
       <c r="C37" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F37" t="s">
         <v>82</v>
@@ -4138,7 +4138,7 @@
         <v>141</v>
       </c>
       <c r="C38" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F38" t="s">
         <v>82</v>
@@ -4200,7 +4200,7 @@
         <v>142</v>
       </c>
       <c r="C39" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F39" t="s">
         <v>82</v>
@@ -4262,7 +4262,7 @@
         <v>143</v>
       </c>
       <c r="C40" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F40" t="s">
         <v>82</v>
@@ -4324,7 +4324,7 @@
         <v>144</v>
       </c>
       <c r="C41" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F41" t="s">
         <v>82</v>
@@ -4386,7 +4386,7 @@
         <v>145</v>
       </c>
       <c r="C42" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F42" t="s">
         <v>82</v>
@@ -4448,7 +4448,7 @@
         <v>146</v>
       </c>
       <c r="C43" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F43" t="s">
         <v>82</v>
@@ -4510,7 +4510,7 @@
         <v>147</v>
       </c>
       <c r="C44" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F44" t="s">
         <v>82</v>
@@ -4572,7 +4572,7 @@
         <v>148</v>
       </c>
       <c r="C45" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F45" t="s">
         <v>82</v>
@@ -4634,7 +4634,7 @@
         <v>149</v>
       </c>
       <c r="C46" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F46" t="s">
         <v>82</v>
@@ -4696,7 +4696,7 @@
         <v>150</v>
       </c>
       <c r="C47" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F47" t="s">
         <v>82</v>
@@ -4758,7 +4758,7 @@
         <v>151</v>
       </c>
       <c r="C48" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F48" t="s">
         <v>82</v>
@@ -4820,7 +4820,7 @@
         <v>152</v>
       </c>
       <c r="C49" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F49" t="s">
         <v>82</v>
@@ -4882,7 +4882,7 @@
         <v>153</v>
       </c>
       <c r="C50" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F50" t="s">
         <v>82</v>
@@ -4944,7 +4944,7 @@
         <v>154</v>
       </c>
       <c r="C51" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F51" t="s">
         <v>82</v>
@@ -5006,7 +5006,7 @@
         <v>155</v>
       </c>
       <c r="C52" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F52" t="s">
         <v>82</v>
@@ -5068,7 +5068,7 @@
         <v>156</v>
       </c>
       <c r="C53" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F53" t="s">
         <v>82</v>
@@ -5124,13 +5124,13 @@
     </row>
     <row r="54" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B54" t="s">
         <v>157</v>
       </c>
       <c r="C54" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F54" t="s">
         <v>82</v>
@@ -5192,7 +5192,7 @@
         <v>158</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F55" s="3" t="s">
         <v>82</v>
@@ -5248,13 +5248,13 @@
     </row>
     <row r="56" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="F56" s="3" t="s">
         <v>82</v>
@@ -5310,13 +5310,13 @@
     </row>
     <row r="57" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F57" s="3" t="s">
         <v>82</v>
@@ -5372,13 +5372,13 @@
     </row>
     <row r="58" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F58" s="3" t="s">
         <v>82</v>
@@ -5434,13 +5434,13 @@
     </row>
     <row r="59" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F59" s="3" t="s">
         <v>82</v>
@@ -5496,13 +5496,13 @@
     </row>
     <row r="60" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F60" s="3" t="s">
         <v>82</v>
@@ -5558,13 +5558,13 @@
     </row>
     <row r="61" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F61" s="3" t="s">
         <v>82</v>
@@ -5620,13 +5620,13 @@
     </row>
     <row r="62" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F62" s="3" t="s">
         <v>82</v>
@@ -5682,13 +5682,13 @@
     </row>
     <row r="63" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F63" s="3" t="s">
         <v>82</v>
@@ -5744,13 +5744,13 @@
     </row>
     <row r="64" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F64" s="3" t="s">
         <v>82</v>
@@ -5806,13 +5806,13 @@
     </row>
     <row r="65" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F65" s="3" t="s">
         <v>82</v>
@@ -5868,13 +5868,13 @@
     </row>
     <row r="66" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F66" s="3" t="s">
         <v>82</v>
@@ -5930,13 +5930,13 @@
     </row>
     <row r="67" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F67" s="3" t="s">
         <v>82</v>
@@ -5992,13 +5992,13 @@
     </row>
     <row r="68" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="F68" s="3" t="s">
         <v>82</v>
@@ -6054,13 +6054,13 @@
     </row>
     <row r="69" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F69" s="3" t="s">
         <v>82</v>
@@ -6119,10 +6119,10 @@
         <v>119</v>
       </c>
       <c r="B70" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C70" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="F70" t="s">
         <v>82</v>
@@ -6178,13 +6178,13 @@
     </row>
     <row r="71" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B71" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C71" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F71" t="s">
         <v>82</v>
@@ -6240,13 +6240,13 @@
     </row>
     <row r="72" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B72" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C72" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F72" t="s">
         <v>82</v>
@@ -6302,13 +6302,13 @@
     </row>
     <row r="73" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B73" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C73" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="F73" t="s">
         <v>82</v>
@@ -6364,13 +6364,13 @@
     </row>
     <row r="74" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B74" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C74" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="F74" t="s">
         <v>82</v>
@@ -6426,13 +6426,13 @@
     </row>
     <row r="75" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B75" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C75" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="F75" t="s">
         <v>82</v>
@@ -6488,13 +6488,13 @@
     </row>
     <row r="76" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B76" t="s">
         <v>120</v>
       </c>
       <c r="C76" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F76" t="s">
         <v>82</v>
@@ -6550,13 +6550,13 @@
     </row>
     <row r="77" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B77" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C77" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F77" t="s">
         <v>82</v>
@@ -6612,13 +6612,13 @@
     </row>
     <row r="78" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B78" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C78" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F78" t="s">
         <v>82</v>
@@ -6674,13 +6674,13 @@
     </row>
     <row r="79" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B79" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C79" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F79" t="s">
         <v>82</v>
@@ -6736,13 +6736,13 @@
     </row>
     <row r="80" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B80" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C80" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F80" t="s">
         <v>82</v>
@@ -6931,13 +6931,13 @@
     </row>
     <row r="83" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B83" t="s">
         <v>121</v>
       </c>
       <c r="C83" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>108</v>
@@ -6996,13 +6996,13 @@
     </row>
     <row r="84" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B84" t="s">
         <v>122</v>
       </c>
       <c r="C84" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>108</v>
@@ -7061,13 +7061,13 @@
     </row>
     <row r="85" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B85" t="s">
         <v>123</v>
       </c>
       <c r="C85" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>108</v>
@@ -7126,13 +7126,13 @@
     </row>
     <row r="86" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B86" t="s">
         <v>124</v>
       </c>
       <c r="C86" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>108</v>
@@ -7191,13 +7191,13 @@
     </row>
     <row r="87" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B87" t="s">
         <v>125</v>
       </c>
       <c r="C87" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>108</v>
@@ -7256,13 +7256,13 @@
     </row>
     <row r="88" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B88" t="s">
         <v>126</v>
       </c>
       <c r="C88" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>108</v>
@@ -7321,13 +7321,13 @@
     </row>
     <row r="89" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B89" t="s">
         <v>127</v>
       </c>
       <c r="C89" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>108</v>
@@ -7386,13 +7386,13 @@
     </row>
     <row r="90" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B90" t="s">
         <v>128</v>
       </c>
       <c r="C90" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>108</v>
@@ -7451,13 +7451,13 @@
     </row>
     <row r="91" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B91" t="s">
         <v>129</v>
       </c>
       <c r="C91" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>108</v>
@@ -7516,13 +7516,13 @@
     </row>
     <row r="92" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B92" t="s">
         <v>130</v>
       </c>
       <c r="C92" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>108</v>
@@ -7581,13 +7581,13 @@
     </row>
     <row r="93" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B93" t="s">
         <v>131</v>
       </c>
       <c r="C93" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>108</v>
@@ -7646,13 +7646,13 @@
     </row>
     <row r="94" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B94" t="s">
         <v>132</v>
       </c>
       <c r="C94" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>108</v>
@@ -7711,13 +7711,13 @@
     </row>
     <row r="95" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B95" t="s">
         <v>133</v>
       </c>
       <c r="C95" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>108</v>
@@ -7776,13 +7776,13 @@
     </row>
     <row r="96" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B96" t="s">
         <v>134</v>
       </c>
       <c r="C96" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>108</v>
@@ -7841,13 +7841,13 @@
     </row>
     <row r="97" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B97" t="s">
         <v>135</v>
       </c>
       <c r="C97" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>108</v>
@@ -7906,13 +7906,13 @@
     </row>
     <row r="98" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B98" t="s">
         <v>136</v>
       </c>
       <c r="C98" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>108</v>
@@ -7971,13 +7971,13 @@
     </row>
     <row r="99" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B99" t="s">
         <v>137</v>
       </c>
       <c r="C99" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D99" s="1" t="s">
         <v>108</v>
@@ -8036,13 +8036,13 @@
     </row>
     <row r="100" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B100" t="s">
         <v>138</v>
       </c>
       <c r="C100" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>108</v>
@@ -8101,13 +8101,13 @@
     </row>
     <row r="101" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B101" t="s">
         <v>139</v>
       </c>
       <c r="C101" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D101" s="1" t="s">
         <v>108</v>
@@ -8166,13 +8166,13 @@
     </row>
     <row r="102" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B102" t="s">
         <v>140</v>
       </c>
       <c r="C102" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>108</v>
@@ -8231,13 +8231,13 @@
     </row>
     <row r="103" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B103" t="s">
         <v>141</v>
       </c>
       <c r="C103" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>108</v>
@@ -8296,13 +8296,13 @@
     </row>
     <row r="104" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B104" t="s">
         <v>142</v>
       </c>
       <c r="C104" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>108</v>
@@ -8361,13 +8361,13 @@
     </row>
     <row r="105" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B105" t="s">
         <v>143</v>
       </c>
       <c r="C105" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>108</v>
@@ -8426,13 +8426,13 @@
     </row>
     <row r="106" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B106" t="s">
         <v>144</v>
       </c>
       <c r="C106" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>108</v>
@@ -8491,13 +8491,13 @@
     </row>
     <row r="107" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B107" t="s">
         <v>145</v>
       </c>
       <c r="C107" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>108</v>
@@ -8556,13 +8556,13 @@
     </row>
     <row r="108" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B108" t="s">
         <v>146</v>
       </c>
       <c r="C108" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>108</v>
@@ -8621,13 +8621,13 @@
     </row>
     <row r="109" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B109" t="s">
         <v>147</v>
       </c>
       <c r="C109" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>108</v>
@@ -8686,13 +8686,13 @@
     </row>
     <row r="110" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B110" t="s">
         <v>148</v>
       </c>
       <c r="C110" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>108</v>
@@ -8751,13 +8751,13 @@
     </row>
     <row r="111" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B111" t="s">
         <v>149</v>
       </c>
       <c r="C111" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>108</v>
@@ -8816,13 +8816,13 @@
     </row>
     <row r="112" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B112" t="s">
         <v>150</v>
       </c>
       <c r="C112" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D112" s="1" t="s">
         <v>108</v>
@@ -8881,13 +8881,13 @@
     </row>
     <row r="113" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B113" t="s">
         <v>151</v>
       </c>
       <c r="C113" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>108</v>
@@ -8946,13 +8946,13 @@
     </row>
     <row r="114" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B114" t="s">
         <v>152</v>
       </c>
       <c r="C114" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>108</v>
@@ -9011,13 +9011,13 @@
     </row>
     <row r="115" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B115" t="s">
         <v>153</v>
       </c>
       <c r="C115" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>108</v>
@@ -9076,13 +9076,13 @@
     </row>
     <row r="116" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B116" t="s">
         <v>154</v>
       </c>
       <c r="C116" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>108</v>
@@ -9141,13 +9141,13 @@
     </row>
     <row r="117" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B117" t="s">
         <v>155</v>
       </c>
       <c r="C117" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>108</v>
@@ -9206,13 +9206,13 @@
     </row>
     <row r="118" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B118" t="s">
         <v>156</v>
       </c>
       <c r="C118" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D118" s="1" t="s">
         <v>108</v>
@@ -9271,13 +9271,13 @@
     </row>
     <row r="119" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B119" t="s">
         <v>157</v>
       </c>
       <c r="C119" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>108</v>
@@ -9336,13 +9336,13 @@
     </row>
     <row r="120" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A120" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B120" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D120" s="5" t="s">
         <v>108</v>
@@ -9401,13 +9401,13 @@
     </row>
     <row r="121" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A121" s="3" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D121" s="5" t="s">
         <v>108</v>
@@ -9466,13 +9466,13 @@
     </row>
     <row r="122" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A122" s="3" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D122" s="5" t="s">
         <v>108</v>
@@ -9531,13 +9531,13 @@
     </row>
     <row r="123" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A123" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D123" s="5" t="s">
         <v>108</v>
@@ -9596,13 +9596,13 @@
     </row>
     <row r="124" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A124" s="3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D124" s="5" t="s">
         <v>108</v>
@@ -9661,13 +9661,13 @@
     </row>
     <row r="125" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A125" s="3" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D125" s="5" t="s">
         <v>108</v>
@@ -9726,13 +9726,13 @@
     </row>
     <row r="126" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A126" s="3" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D126" s="5" t="s">
         <v>108</v>
@@ -9791,13 +9791,13 @@
     </row>
     <row r="127" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A127" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D127" s="5" t="s">
         <v>108</v>
@@ -9856,13 +9856,13 @@
     </row>
     <row r="128" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A128" s="3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D128" s="5" t="s">
         <v>108</v>
@@ -9921,13 +9921,13 @@
     </row>
     <row r="129" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A129" s="3" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D129" s="5" t="s">
         <v>108</v>
@@ -9986,13 +9986,13 @@
     </row>
     <row r="130" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A130" s="3" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D130" s="5" t="s">
         <v>108</v>
@@ -10051,13 +10051,13 @@
     </row>
     <row r="131" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A131" s="3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C131" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D131" s="5" t="s">
         <v>108</v>
@@ -10116,13 +10116,13 @@
     </row>
     <row r="132" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A132" s="3" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D132" s="5" t="s">
         <v>108</v>
@@ -10181,13 +10181,13 @@
     </row>
     <row r="133" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A133" s="3" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D133" s="5" t="s">
         <v>108</v>
@@ -10246,13 +10246,13 @@
     </row>
     <row r="134" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A134" s="3" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D134" s="5" t="s">
         <v>108</v>
@@ -10314,7 +10314,7 @@
         <v>159</v>
       </c>
       <c r="B135" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C135" t="s">
         <v>160</v>
@@ -10376,13 +10376,13 @@
     </row>
     <row r="136" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
+        <v>402</v>
+      </c>
+      <c r="B136" t="s">
+        <v>365</v>
+      </c>
+      <c r="C136" t="s">
         <v>403</v>
-      </c>
-      <c r="B136" t="s">
-        <v>366</v>
-      </c>
-      <c r="C136" t="s">
-        <v>404</v>
       </c>
       <c r="D136" s="1" t="s">
         <v>108</v>
@@ -10441,13 +10441,13 @@
     </row>
     <row r="137" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
+        <v>404</v>
+      </c>
+      <c r="B137" t="s">
+        <v>366</v>
+      </c>
+      <c r="C137" t="s">
         <v>405</v>
-      </c>
-      <c r="B137" t="s">
-        <v>367</v>
-      </c>
-      <c r="C137" t="s">
-        <v>406</v>
       </c>
       <c r="D137" s="1" t="s">
         <v>108</v>
@@ -10506,13 +10506,13 @@
     </row>
     <row r="138" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
+        <v>406</v>
+      </c>
+      <c r="B138" t="s">
+        <v>367</v>
+      </c>
+      <c r="C138" t="s">
         <v>407</v>
-      </c>
-      <c r="B138" t="s">
-        <v>368</v>
-      </c>
-      <c r="C138" t="s">
-        <v>408</v>
       </c>
       <c r="D138" s="1" t="s">
         <v>108</v>
@@ -10571,13 +10571,13 @@
     </row>
     <row r="139" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
+        <v>408</v>
+      </c>
+      <c r="B139" t="s">
+        <v>368</v>
+      </c>
+      <c r="C139" t="s">
         <v>409</v>
-      </c>
-      <c r="B139" t="s">
-        <v>369</v>
-      </c>
-      <c r="C139" t="s">
-        <v>410</v>
       </c>
       <c r="D139" s="1" t="s">
         <v>108</v>
@@ -10636,13 +10636,13 @@
     </row>
     <row r="140" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
+        <v>410</v>
+      </c>
+      <c r="B140" t="s">
+        <v>369</v>
+      </c>
+      <c r="C140" t="s">
         <v>411</v>
-      </c>
-      <c r="B140" t="s">
-        <v>370</v>
-      </c>
-      <c r="C140" t="s">
-        <v>412</v>
       </c>
       <c r="D140" s="1" t="s">
         <v>108</v>
@@ -10701,13 +10701,13 @@
     </row>
     <row r="141" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B141" t="s">
         <v>120</v>
       </c>
       <c r="C141" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D141" s="1" t="s">
         <v>108</v>
@@ -10766,13 +10766,13 @@
     </row>
     <row r="142" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
+        <v>414</v>
+      </c>
+      <c r="B142" t="s">
+        <v>370</v>
+      </c>
+      <c r="C142" t="s">
         <v>415</v>
-      </c>
-      <c r="B142" t="s">
-        <v>371</v>
-      </c>
-      <c r="C142" t="s">
-        <v>416</v>
       </c>
       <c r="D142" s="1" t="s">
         <v>108</v>
@@ -10831,13 +10831,13 @@
     </row>
     <row r="143" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
+        <v>416</v>
+      </c>
+      <c r="B143" t="s">
+        <v>371</v>
+      </c>
+      <c r="C143" t="s">
         <v>417</v>
-      </c>
-      <c r="B143" t="s">
-        <v>372</v>
-      </c>
-      <c r="C143" t="s">
-        <v>418</v>
       </c>
       <c r="D143" s="1" t="s">
         <v>108</v>
@@ -10896,13 +10896,13 @@
     </row>
     <row r="144" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
+        <v>418</v>
+      </c>
+      <c r="B144" t="s">
+        <v>372</v>
+      </c>
+      <c r="C144" t="s">
         <v>419</v>
-      </c>
-      <c r="B144" t="s">
-        <v>373</v>
-      </c>
-      <c r="C144" t="s">
-        <v>420</v>
       </c>
       <c r="D144" s="1" t="s">
         <v>108</v>
@@ -10961,13 +10961,13 @@
     </row>
     <row r="145" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
+        <v>420</v>
+      </c>
+      <c r="B145" t="s">
+        <v>373</v>
+      </c>
+      <c r="C145" t="s">
         <v>421</v>
-      </c>
-      <c r="B145" t="s">
-        <v>374</v>
-      </c>
-      <c r="C145" t="s">
-        <v>422</v>
       </c>
       <c r="D145" s="1" t="s">
         <v>108</v>

</xml_diff>